<commit_message>
Changed The Price Calculator and Price List
</commit_message>
<xml_diff>
--- a/Price List.xlsx
+++ b/Price List.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Price List" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -474,7 +474,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>